<commit_message>
Droit de mutation dans spécification
</commit_message>
<xml_diff>
--- a/spécification.xlsx
+++ b/spécification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="980" yWindow="80" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="montage financier" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t xml:space="preserve">Hypothèque  </t>
   </si>
@@ -92,14 +92,76 @@
     <t>http://www.domdomotique.com/product</t>
   </si>
   <si>
-    <t>lumièere extérieure</t>
+    <t>lumière extérieure</t>
+  </si>
+  <si>
+    <t>vérifier quand ikea spéciaux 20% cuisine au Canada</t>
+  </si>
+  <si>
+    <t>terrain Robert</t>
+  </si>
+  <si>
+    <t>terrain Boutin</t>
+  </si>
+  <si>
+    <t>Bienvenue Robert</t>
+  </si>
+  <si>
+    <t>Bienvenue totale</t>
+  </si>
+  <si>
+    <t>Bienvenue Boutin</t>
+  </si>
+  <si>
+    <t>H-1</t>
+  </si>
+  <si>
+    <t>H-2</t>
+  </si>
+  <si>
+    <t>H-3</t>
+  </si>
+  <si>
+    <t>H-4</t>
+  </si>
+  <si>
+    <t>H-5</t>
+  </si>
+  <si>
+    <t>Achat au prix de l'évaluation</t>
+  </si>
+  <si>
+    <t>Achat au prix réel tout mis sur le terrain de M. Boutin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achat au prix réel et le montant est proportionné selon l'évaluation de chaque terrain </t>
+  </si>
+  <si>
+    <t>Achat au prix réel et le prix d'achat du terrain de Mme Robert à 50 000$</t>
+  </si>
+  <si>
+    <t>Comme H-4 mais au prix total de 315 000$</t>
+  </si>
+  <si>
+    <t>Droit de mutation - Taxe de Bienvenue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,6 +185,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,21 +211,75 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="26">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -484,68 +608,342 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
         <v>97500</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="2"/>
+      <c r="E4" s="3">
+        <f>5/1000</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2">
         <v>13000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="2"/>
+      <c r="E5" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="2">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
         <v>81000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="2"/>
+      <c r="E6" s="3">
+        <f>1.5/100</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
+        <v>110000</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
         <v>10000</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="C12">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
         <f>SUM(C4:C8)</f>
-        <v>301500</v>
+        <v>311500</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" s="4" customFormat="1">
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2">
+        <v>21632</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
+        <f>C20/B20 *B19</f>
+        <v>32791.044776119401</v>
+      </c>
+      <c r="E19" s="2">
+        <v>50000</v>
+      </c>
+      <c r="F19" s="2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="2">
+        <v>214400</v>
+      </c>
+      <c r="C20" s="2">
+        <v>325000</v>
+      </c>
+      <c r="D20" s="2">
+        <f>C20-D19</f>
+        <v>292208.95522388059</v>
+      </c>
+      <c r="E20" s="2">
+        <v>275000</v>
+      </c>
+      <c r="F20" s="2">
+        <v>265000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2">
+        <f>B19 *$E4</f>
+        <v>108.16</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
+        <f>D19 *$E4</f>
+        <v>163.955223880597</v>
+      </c>
+      <c r="E22" s="2">
+        <f>E19 *$E4</f>
+        <v>250</v>
+      </c>
+      <c r="F22" s="2">
+        <f>F19 *$E4</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="2">
+        <f>($E4 *$F4) + (B20 -$F4) *$E5</f>
+        <v>1894</v>
+      </c>
+      <c r="C23" s="2">
+        <f>($E4 *$F4) + (C20 -$F4) *$E5</f>
+        <v>3000</v>
+      </c>
+      <c r="D23" s="2">
+        <f>($E4 *$F4) + (D20 -$F4) * $E5</f>
+        <v>2672.0895522388059</v>
+      </c>
+      <c r="E23" s="2">
+        <f>($E4 *$F4) + (E20 -$F4) * $E5</f>
+        <v>2500</v>
+      </c>
+      <c r="F23" s="2">
+        <f>($E4 *$F4) + (F20 -$F4) * $E5</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2">
+        <f>B22+B23</f>
+        <v>2002.16</v>
+      </c>
+      <c r="C24" s="2">
+        <f>C22+C23</f>
+        <v>3000</v>
+      </c>
+      <c r="D24" s="2">
+        <f>D22+D23</f>
+        <v>2836.0447761194027</v>
+      </c>
+      <c r="E24" s="2">
+        <f>E22+E23</f>
+        <v>2750</v>
+      </c>
+      <c r="F24" s="2">
+        <f>F22+F23</f>
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -612,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A12:A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -679,6 +1077,11 @@
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
domotique et droit de passage
</commit_message>
<xml_diff>
--- a/spécification.xlsx
+++ b/spécification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="montage financier" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t xml:space="preserve">Hypothèque  </t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>Droit de mutation - Taxe de Bienvenue</t>
+  </si>
+  <si>
+    <t>http://www.digitaltrends.com/home/zigbee-vs-zwave-vs-insteon-home-automation-protocols-explained/#ixzz3xL6rNmK2</t>
+  </si>
+  <si>
+    <t>protocoles</t>
+  </si>
+  <si>
+    <t>Logiciel</t>
+  </si>
+  <si>
+    <t>openhab</t>
   </si>
 </sst>
 </file>
@@ -614,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1014,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1086,6 +1098,31 @@
     <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
offre d'achat signé et négatif
</commit_message>
<xml_diff>
--- a/spécification.xlsx
+++ b/spécification.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="montage financier" sheetId="1" r:id="rId1"/>
     <sheet name="question" sheetId="2" r:id="rId2"/>
     <sheet name="spécification" sheetId="3" r:id="rId3"/>
+    <sheet name="domoti" sheetId="4" r:id="rId4"/>
+    <sheet name="contacts" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t xml:space="preserve">Hypothèque  </t>
   </si>
@@ -156,6 +158,96 @@
   </si>
   <si>
     <t>openhab</t>
+  </si>
+  <si>
+    <t>Thermostat</t>
+  </si>
+  <si>
+    <t>Nest</t>
+  </si>
+  <si>
+    <t>note : Ces sont des thermostats qui fonctionne avec le 24 volt</t>
+  </si>
+  <si>
+    <t>site web intéressant</t>
+  </si>
+  <si>
+    <t>smartthome.com</t>
+  </si>
+  <si>
+    <t>Caméra</t>
+  </si>
+  <si>
+    <t>netatmo</t>
+  </si>
+  <si>
+    <t>nest</t>
+  </si>
+  <si>
+    <t>spypoint</t>
+  </si>
+  <si>
+    <t>caleo</t>
+  </si>
+  <si>
+    <t>Station météo</t>
+  </si>
+  <si>
+    <t>homeremote</t>
+  </si>
+  <si>
+    <t>protocole</t>
+  </si>
+  <si>
+    <t>zigbee</t>
+  </si>
+  <si>
+    <t>zwave</t>
+  </si>
+  <si>
+    <t>2.4 gh</t>
+  </si>
+  <si>
+    <t>900 mh</t>
+  </si>
+  <si>
+    <t>casaconnect quebecois mais pas recommandé</t>
+  </si>
+  <si>
+    <t>note : privilégié  zigbee</t>
+  </si>
+  <si>
+    <t>produit domotique</t>
+  </si>
+  <si>
+    <t>Boite électrique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TED permet d'avoir des infos sur sa consommation </t>
+  </si>
+  <si>
+    <t>insteon</t>
+  </si>
+  <si>
+    <t>utiliser un relais ppur plinthe électrique (30$)</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>IFTT</t>
+  </si>
+  <si>
+    <t>wemo  protoclole upnp(wallmart) LUMIÈRE PRISE ETC ..</t>
+  </si>
+  <si>
+    <t>ecobee</t>
+  </si>
+  <si>
+    <t>Locataire à Claude : Gypse</t>
   </si>
 </sst>
 </file>
@@ -223,11 +315,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -267,7 +363,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="32">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="6" builtinId="8" hidden="1"/>
@@ -281,6 +377,8 @@
     <cellStyle name="Lien hypertexte" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
@@ -294,6 +392,8 @@
     <cellStyle name="Lien hypertexte visité" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="3" builtinId="5"/>
   </cellStyles>
@@ -1028,7 +1128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -1123,6 +1223,199 @@
     <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>